<commit_message>
final version presentation results
</commit_message>
<xml_diff>
--- a/Energy community potential model/_inputs.xlsx
+++ b/Energy community potential model/_inputs.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Energy-community-potential-model\Energy community potential model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FEE2061-1361-4D3E-A598-F6BDA09EB429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E54075A-BCBC-45D6-8799-55A0A2988808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B6C73CCE-982B-4A1F-9730-EB531FF2A0F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B6C73CCE-982B-4A1F-9730-EB531FF2A0F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>base case</t>
   </si>
@@ -69,6 +71,12 @@
   </si>
   <si>
     <t>SMALL_SCALE_SIMILAR</t>
+  </si>
+  <si>
+    <t>Bit slow in uptake</t>
+  </si>
+  <si>
+    <t>Not enough projects fo learnng</t>
   </si>
 </sst>
 </file>
@@ -121,6 +129,549 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>188368</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>113202</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2CA4CC2-3FD2-C02C-8E8B-77441F6B19AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2377440"/>
+          <a:ext cx="12022228" cy="5782482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>592249</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>118969</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{269CA177-C099-705C-0E3E-40F87112AF95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13053060" y="2560320"/>
+          <a:ext cx="12174649" cy="6154009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>179966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>588922</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>2261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948216C9-B260-EFA2-2298-9EFA5BB30A96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7799966"/>
+          <a:ext cx="12418972" cy="7823295"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>235527</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>83128</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>189597</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>18164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DD9108-0BAE-5461-281F-4CCD8E664CBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12676909" y="8908473"/>
+          <a:ext cx="12146070" cy="6058746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>239775</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>58879</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D692FAC-2D15-DEB4-0A35-513D6817B403}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11822175" cy="6182588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>401782</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>166255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>165325</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>22407</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3930C14F-20AB-D638-5BC0-1608186A7AD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12593782" y="166255"/>
+          <a:ext cx="11955543" cy="5439534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>221673</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>13854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>4269</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>30172</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBDD9E34-51A1-268E-BCD8-870CBD40C432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12413673" y="5597236"/>
+          <a:ext cx="11974596" cy="5239481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>468407</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>128851</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19ABFEDE-AD8F-A352-A192-6C38821F5646}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6303818"/>
+          <a:ext cx="12050807" cy="4991797"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>96965</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>90262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{402B7AB9-5040-44F4-6ED7-65F0F60383F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12288965" cy="5210902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>239486</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>144563</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE455198-4D72-53E6-0E5B-351B0A492DC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="239486" y="3276600"/>
+          <a:ext cx="2343477" cy="3323595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>174172</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>604473</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EEEA3F2-ECE0-DCAC-4AA0-FD365D94A3B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11756572" y="0"/>
+          <a:ext cx="12012701" cy="5391902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>370114</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>114605</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>172229</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7026D363-9BE5-9664-9F73-FDEC1DEC725C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8294914" y="4767943"/>
+          <a:ext cx="11936491" cy="5582429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,18 +991,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92774EF-C57A-4676-B264-7782667611B0}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E7"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -465,47 +1016,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>0.71</v>
       </c>
+      <c r="C2">
+        <v>0.71</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.65</v>
+        <v>0.66</v>
+      </c>
+      <c r="C3">
+        <v>0.66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <v>0.7</v>
       </c>
+      <c r="C4">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.01</v>
       </c>
+      <c r="C6">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -520,9 +1086,50 @@
       </c>
       <c r="E7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0BE3FA1-F110-4E60-A327-4DB7906BAF51}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1F0D09-F37B-4BCA-BC0F-FA2F83222376}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>